<commit_message>
add full words of each language into the matrix
</commit_message>
<xml_diff>
--- a/test/3lines.xlsx
+++ b/test/3lines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jan/dev/prive/tessa/alignement_cognats/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAC49CD-A268-0847-ABA0-C300E51633D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AEC2A1-BF81-9843-8EEA-08B77EC8AB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8080" yWindow="8720" windowWidth="27640" windowHeight="16940" xr2:uid="{8346597E-EC61-6445-BAFB-F8065F92FFE6}"/>
   </bookViews>
@@ -575,9 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5FBDE8-BC74-C246-8E23-493BBCF01209}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>

</xml_diff>